<commit_message>
Add more User Stories
</commit_message>
<xml_diff>
--- a/Antrag/User Stories.xlsx
+++ b/Antrag/User Stories.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rasidbajramov/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rasidbajramov/Library/Mobile Documents/com~apple~CloudDocs/simplydone/Antrag/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7E5D992-B861-0C43-8676-41036DFCC9CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81FA03D5-34E9-5B4B-BC33-DFBA1A5A0615}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="480" windowWidth="28800" windowHeight="17520" xr2:uid="{6E36DC40-5F18-4EBE-9BC3-7D855008A313}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="70">
   <si>
     <t>Priority scale</t>
   </si>
@@ -192,6 +192,60 @@
   </si>
   <si>
     <t>Button: 'Aufgabe hinzufügen', 'Korrigieren', 'Löschen' Checkbox 'Aufgabe erledigt'</t>
+  </si>
+  <si>
+    <t>Product Goal 7 - Desktop-App</t>
+  </si>
+  <si>
+    <t>möchte Fälligkeitsdatum eintragen</t>
+  </si>
+  <si>
+    <t>um ein zeitlichen Überblick haben</t>
+  </si>
+  <si>
+    <t>Select Menu</t>
+  </si>
+  <si>
+    <t>Product Goal 7 - Web- App</t>
+  </si>
+  <si>
+    <t xml:space="preserve">möchte Priorität eintragen </t>
+  </si>
+  <si>
+    <t>Product Goal 8 - Desktop-App</t>
+  </si>
+  <si>
+    <t>um die Arbeitszeit zu organisieren</t>
+  </si>
+  <si>
+    <t>Product Goal 9 - Web-App</t>
+  </si>
+  <si>
+    <t>Product Goal 10 - Desktop-App</t>
+  </si>
+  <si>
+    <t>möchte Dashboard anpassen und Widgets mit eigenen Filter erstellen</t>
+  </si>
+  <si>
+    <t>um die Darstellung anzupassen</t>
+  </si>
+  <si>
+    <t>Filter</t>
+  </si>
+  <si>
+    <t>Product Goal 10 - Desktop-Web</t>
+  </si>
+  <si>
+    <t>Product Goal 11 - Desktop-App</t>
+  </si>
+  <si>
+    <t>möchte meine Kategorien mit anderen Benutzern teilen</t>
+  </si>
+  <si>
+    <t>um gemeinsam To.Do's zu erstellen</t>
+  </si>
+  <si>
+    <t>DB, Share-Button</t>
   </si>
 </sst>
 </file>
@@ -271,7 +325,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -282,11 +336,48 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="23">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment wrapText="1"/>
     </dxf>
@@ -337,20 +428,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{35383E86-7FBF-4BC5-A1FB-8B8878744FCB}" name="Tabelle1" displayName="Tabelle1" ref="C3:M20" totalsRowShown="0" dataDxfId="11">
-  <autoFilter ref="C3:M20" xr:uid="{35383E86-7FBF-4BC5-A1FB-8B8878744FCB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{35383E86-7FBF-4BC5-A1FB-8B8878744FCB}" name="Tabelle1" displayName="Tabelle1" ref="C3:M22" totalsRowCount="1" dataDxfId="22">
+  <autoFilter ref="C3:M21" xr:uid="{35383E86-7FBF-4BC5-A1FB-8B8878744FCB}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{25C8B47E-6BAC-4926-B248-911D3C771B26}" name="Priority" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{9CE9A60A-229A-4767-BF36-858767E4CC66}" name="BusinessValue" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{3A030762-622D-4E41-9B8E-D710A45689B2}" name="Product Goal" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{8E256A41-5702-4745-B9E8-A17D429DF600}" name="Theme" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{CFB4564A-616C-4819-9D7C-AC6BA5930B49}" name="US_ID" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{BE11ABC0-35C9-4FDA-AEDC-7DFC4279495F}" name="As a…" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{0A30299E-AA3D-4857-8377-225ADFB10DEA}" name="I want to be able to …" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{BC54D1C0-A767-4AA9-9D83-23DDBA33D135}" name="So that…" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{09C01375-324D-4B4B-905F-C1021C7749D5}" name="StoryPoint" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{62F087AF-479D-4C5D-9AD4-902DF4124D3B}" name="Estimates (hours)" dataDxfId="1"/>
-    <tableColumn id="11" xr3:uid="{D45FF381-DA23-4472-8A72-DFADF546D694}" name="Acceptance Criteria" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{25C8B47E-6BAC-4926-B248-911D3C771B26}" name="Priority" dataDxfId="21" totalsRowDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{9CE9A60A-229A-4767-BF36-858767E4CC66}" name="BusinessValue" dataDxfId="20" totalsRowDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{3A030762-622D-4E41-9B8E-D710A45689B2}" name="Product Goal" dataDxfId="19" totalsRowDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{8E256A41-5702-4745-B9E8-A17D429DF600}" name="Theme" dataDxfId="18" totalsRowDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{CFB4564A-616C-4819-9D7C-AC6BA5930B49}" name="US_ID" dataDxfId="17" totalsRowDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{BE11ABC0-35C9-4FDA-AEDC-7DFC4279495F}" name="As a…" dataDxfId="16" totalsRowDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{0A30299E-AA3D-4857-8377-225ADFB10DEA}" name="I want to be able to …" dataDxfId="15" totalsRowDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{BC54D1C0-A767-4AA9-9D83-23DDBA33D135}" name="So that…" dataDxfId="14" totalsRowDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{09C01375-324D-4B4B-905F-C1021C7749D5}" name="StoryPoint" dataDxfId="13" totalsRowDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{62F087AF-479D-4C5D-9AD4-902DF4124D3B}" name="Estimates (hours)" totalsRowFunction="sum" dataDxfId="12" totalsRowDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{D45FF381-DA23-4472-8A72-DFADF546D694}" name="Acceptance Criteria" dataDxfId="11" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -653,10 +744,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E7C2921-B808-43C3-9286-7C3D73229528}">
-  <dimension ref="C1:M20"/>
+  <dimension ref="C1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D3" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" topLeftCell="D12" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -844,10 +935,10 @@
         <v>27</v>
       </c>
       <c r="K6" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L6" s="5">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="M6" s="5" t="s">
         <v>28</v>
@@ -879,10 +970,10 @@
         <v>27</v>
       </c>
       <c r="K7" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L7" s="5">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="M7" s="5" t="s">
         <v>28</v>
@@ -914,10 +1005,10 @@
         <v>30</v>
       </c>
       <c r="K8" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L8" s="5">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="M8" s="5" t="s">
         <v>31</v>
@@ -952,7 +1043,7 @@
         <v>5</v>
       </c>
       <c r="L9" s="5">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="M9" s="5" t="s">
         <v>36</v>
@@ -987,7 +1078,7 @@
         <v>5</v>
       </c>
       <c r="L10" s="5">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="M10" s="5" t="s">
         <v>36</v>
@@ -1019,10 +1110,10 @@
         <v>38</v>
       </c>
       <c r="K11" s="5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="L11" s="5">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="M11" s="5" t="s">
         <v>39</v>
@@ -1054,9 +1145,11 @@
         <v>38</v>
       </c>
       <c r="K12" s="5">
-        <v>2</v>
-      </c>
-      <c r="L12" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="L12" s="5">
+        <v>5</v>
+      </c>
       <c r="M12" s="5" t="s">
         <v>39</v>
       </c>
@@ -1087,10 +1180,10 @@
         <v>50</v>
       </c>
       <c r="K13" s="5">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="L13" s="5">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="M13" s="5" t="s">
         <v>51</v>
@@ -1122,93 +1215,282 @@
         <v>50</v>
       </c>
       <c r="K14" s="5">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="L14" s="5">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="M14" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="3:13" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-    </row>
-    <row r="16" spans="3:13" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
-    </row>
-    <row r="17" spans="3:13" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-    </row>
-    <row r="18" spans="3:13" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-    </row>
-    <row r="19" spans="3:13" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
-    </row>
-    <row r="20" spans="3:13" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
+    <row r="15" spans="3:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="C15" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="5">
+        <v>3</v>
+      </c>
+      <c r="E15" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G15" s="5">
+        <v>12</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="K15" s="5">
+        <v>2</v>
+      </c>
+      <c r="L15" s="5">
+        <v>2</v>
+      </c>
+      <c r="M15" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="3:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="C16" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="5">
+        <v>3</v>
+      </c>
+      <c r="E16" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16" s="5">
+        <v>13</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="K16" s="5">
+        <v>2</v>
+      </c>
+      <c r="L16" s="5">
+        <v>2</v>
+      </c>
+      <c r="M16" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="3:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="C17" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="5">
+        <v>3</v>
+      </c>
+      <c r="E17" t="s">
+        <v>58</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G17" s="5">
+        <v>14</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I17" t="s">
+        <v>57</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="K17" s="5">
+        <v>2</v>
+      </c>
+      <c r="L17" s="5">
+        <v>2</v>
+      </c>
+      <c r="M17" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="3:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="C18" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" s="5">
+        <v>3</v>
+      </c>
+      <c r="E18" t="s">
+        <v>60</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G18" s="5">
+        <v>15</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I18" t="s">
+        <v>57</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="K18" s="5">
+        <v>2</v>
+      </c>
+      <c r="L18" s="5">
+        <v>2</v>
+      </c>
+      <c r="M18" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="3:13" ht="48" x14ac:dyDescent="0.2">
+      <c r="C19" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="5">
+        <v>2</v>
+      </c>
+      <c r="E19" t="s">
+        <v>61</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G19" s="5">
+        <v>16</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J19" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="K19" s="5">
+        <v>5</v>
+      </c>
+      <c r="L19" s="5">
+        <v>8</v>
+      </c>
+      <c r="M19" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="3:13" ht="48" x14ac:dyDescent="0.2">
+      <c r="C20" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="5">
+        <v>2</v>
+      </c>
+      <c r="E20" t="s">
+        <v>65</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G20" s="5">
+        <v>17</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J20" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="K20" s="5">
+        <v>5</v>
+      </c>
+      <c r="L20" s="5">
+        <v>8</v>
+      </c>
+      <c r="M20" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="3:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="C21" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" s="5">
+        <v>4</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G21" s="5">
+        <v>18</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="J21" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="K21" s="5">
+        <v>13</v>
+      </c>
+      <c r="L21" s="5">
+        <v>13</v>
+      </c>
+      <c r="M21" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5">
+        <f>SUBTOTAL(109,Tabelle1[Estimates (hours)])</f>
+        <v>94</v>
+      </c>
+      <c r="M22" s="5"/>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C20" xr:uid="{0C4E6ECF-68E6-4C69-84EC-B67BB79105BC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C21" xr:uid="{0C4E6ECF-68E6-4C69-84EC-B67BB79105BC}">
       <formula1>$D$1:$G$1</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:D20" xr:uid="{CC98014D-015B-493D-AA10-1DCCCD92FE62}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:D21" xr:uid="{CC98014D-015B-493D-AA10-1DCCCD92FE62}">
       <formula1>$D$2:$G$2</formula1>
     </dataValidation>
   </dataValidations>
@@ -1221,18 +1503,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0ba74dc7-3b53-4713-bb67-9e6187bc4572">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <a xmlns="0ba74dc7-3b53-4713-bb67-9e6187bc4572" xsi:nil="true"/>
-    <TaxCatchAll xmlns="b43d7674-e72d-422b-be95-e22e3af49d99" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101006B8247937E6F6047838B253C0692F937" ma:contentTypeVersion="9" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="c4b8eaee6a81220e587889abe47f8d5a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0ba74dc7-3b53-4713-bb67-9e6187bc4572" xmlns:ns3="b43d7674-e72d-422b-be95-e22e3af49d99" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="adbd04a2623e67f13a6436da20248267" ns2:_="" ns3:_="">
     <xsd:import namespace="0ba74dc7-3b53-4713-bb67-9e6187bc4572"/>
@@ -1417,6 +1687,18 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0ba74dc7-3b53-4713-bb67-9e6187bc4572">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <a xmlns="0ba74dc7-3b53-4713-bb67-9e6187bc4572" xsi:nil="true"/>
+    <TaxCatchAll xmlns="b43d7674-e72d-422b-be95-e22e3af49d99" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1427,17 +1709,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE5B2139-0411-4F93-927B-CEF9303A0586}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="0ba74dc7-3b53-4713-bb67-9e6187bc4572"/>
-    <ds:schemaRef ds:uri="b43d7674-e72d-422b-be95-e22e3af49d99"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7B1011D-8939-4CDB-887E-5FE3CE1D8589}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1456,6 +1727,17 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE5B2139-0411-4F93-927B-CEF9303A0586}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="0ba74dc7-3b53-4713-bb67-9e6187bc4572"/>
+    <ds:schemaRef ds:uri="b43d7674-e72d-422b-be95-e22e3af49d99"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3CD4954-40DF-4E1B-A417-8AC111E78ABB}">
   <ds:schemaRefs>

</xml_diff>